<commit_message>
add 1409 1877 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -653,7 +653,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -673,7 +673,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -710,7 +710,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -730,7 +730,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -767,7 +767,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -787,7 +787,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -824,7 +824,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -844,7 +844,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -881,7 +881,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -901,7 +901,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1093,6 +1093,82 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="152400" y="1371600"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>369967</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>198517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="图片 12"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="180975" y="1609725"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>389017</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>360442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="图片 13"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="200025" y="1990725"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1393,7 +1469,7 @@
   <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
add 2001 1264 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -653,7 +653,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -673,7 +673,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -710,7 +710,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -730,7 +730,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -767,7 +767,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -787,7 +787,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -824,7 +824,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -844,7 +844,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -881,7 +881,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -901,7 +901,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1169,6 +1169,82 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="200025" y="1990725"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>379492</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>341392</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="图片 14"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="2343150"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>398542</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>217567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="图片 15"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="209550" y="2590800"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1468,8 +1544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
add 1319 1567 1581 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="20730" windowHeight="9645"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -505,8 +505,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -552,6 +552,12 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8.9"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -606,7 +612,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -624,6 +630,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -668,7 +677,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -688,7 +697,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -725,7 +734,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -745,7 +754,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -782,7 +791,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -802,7 +811,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -839,7 +848,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -859,7 +868,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -896,7 +905,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -916,7 +925,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1763,11 +1772,125 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>417592</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>350917</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="图片 29"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="7381875"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>408067</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>217567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="图片 30"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="219075" y="7620000"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>379492</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>208042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="图片 31"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="7829550"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1841,6 +1964,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1875,6 +1999,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2050,11 +2175,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2557,6 +2682,9 @@
       </c>
       <c r="F26" s="2">
         <v>43</v>
+      </c>
+      <c r="G26" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="17.25" thickBot="1">
@@ -4018,20 +4146,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D47" sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="4:4">
+      <c r="D1" s="6"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add 1263 1991 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -1915,6 +1915,82 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="171450" y="8181975"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>360442</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>17542</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="图片 33"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="8448675"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>331867</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>360442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="35" name="图片 34"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="142875" y="8791575"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2217,7 +2293,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
add 1100 1327 1876 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -1991,6 +1991,120 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="142875" y="8791575"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>379492</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>360442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="36" name="图片 35"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="9163050"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>360442</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>208042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="37" name="图片 36"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="9382125"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>360442</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>360442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="38" name="图片 37"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="9753600"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2293,7 +2407,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2890,6 +3004,9 @@
       <c r="F31" s="2">
         <v>50</v>
       </c>
+      <c r="G31" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="17.25" thickBot="1">
       <c r="A32" s="2"/>
@@ -2909,7 +3026,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="29.25" thickBot="1">
+    <row r="33" spans="1:7" ht="29.25" thickBot="1">
       <c r="A33" s="2"/>
       <c r="B33" s="2">
         <v>1876</v>
@@ -2926,8 +3043,11 @@
       <c r="F33" s="2">
         <v>52</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="27.75" thickBot="1">
+      <c r="G33" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="27.75" thickBot="1">
       <c r="A34" s="2"/>
       <c r="B34" s="2">
         <v>1243</v>
@@ -2945,7 +3065,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17.25" thickBot="1">
+    <row r="35" spans="1:7" ht="17.25" thickBot="1">
       <c r="A35" s="2"/>
       <c r="B35" s="2">
         <v>1493</v>
@@ -2963,7 +3083,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="29.25" thickBot="1">
+    <row r="36" spans="1:7" ht="29.25" thickBot="1">
       <c r="A36" s="2"/>
       <c r="B36" s="2">
         <v>1110</v>
@@ -2981,7 +3101,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="17.25" thickBot="1">
+    <row r="37" spans="1:7" ht="17.25" thickBot="1">
       <c r="A37" s="2"/>
       <c r="B37" s="2">
         <v>1349</v>
@@ -2999,7 +3119,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="17.25" thickBot="1">
+    <row r="38" spans="1:7" ht="17.25" thickBot="1">
       <c r="A38" s="2"/>
       <c r="B38" s="2">
         <v>1607</v>
@@ -3017,7 +3137,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="29.25" thickBot="1">
+    <row r="39" spans="1:7" ht="29.25" thickBot="1">
       <c r="A39" s="2"/>
       <c r="B39" s="2">
         <v>1881</v>
@@ -3035,7 +3155,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="29.25" thickBot="1">
+    <row r="40" spans="1:7" ht="29.25" thickBot="1">
       <c r="A40" s="2"/>
       <c r="B40" s="2">
         <v>1893</v>
@@ -3053,7 +3173,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="17.25" thickBot="1">
+    <row r="41" spans="1:7" ht="17.25" thickBot="1">
       <c r="A41" s="2"/>
       <c r="B41" s="2">
         <v>1545</v>
@@ -3071,7 +3191,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="17.25" thickBot="1">
+    <row r="42" spans="1:7" ht="17.25" thickBot="1">
       <c r="A42" s="2"/>
       <c r="B42" s="2">
         <v>1496</v>
@@ -3089,7 +3209,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="17.25" thickBot="1">
+    <row r="43" spans="1:7" ht="17.25" thickBot="1">
       <c r="A43" s="2"/>
       <c r="B43" s="2">
         <v>1196</v>
@@ -3107,7 +3227,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="17.25" thickBot="1">
+    <row r="44" spans="1:7" ht="17.25" thickBot="1">
       <c r="A44" s="2"/>
       <c r="B44" s="2">
         <v>1636</v>
@@ -3125,7 +3245,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="17.25" thickBot="1">
+    <row r="45" spans="1:7" ht="17.25" thickBot="1">
       <c r="A45" s="2"/>
       <c r="B45" s="2">
         <v>1837</v>
@@ -3143,7 +3263,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="29.25" thickBot="1">
+    <row r="46" spans="1:7" ht="29.25" thickBot="1">
       <c r="A46" s="2"/>
       <c r="B46" s="2">
         <v>1925</v>
@@ -3161,7 +3281,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="17.25" thickBot="1">
+    <row r="47" spans="1:7" ht="17.25" thickBot="1">
       <c r="A47" s="2"/>
       <c r="B47" s="2">
         <v>1149</v>
@@ -3177,7 +3297,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="17.25" thickBot="1">
+    <row r="48" spans="1:7" ht="17.25" thickBot="1">
       <c r="A48" s="2"/>
       <c r="B48" s="2">
         <v>1563</v>

</xml_diff>

<commit_message>
add 1243 1493 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="160">
   <si>
     <t>ID</t>
   </si>
@@ -2105,6 +2105,82 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="171450" y="9753600"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>360442</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>198517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="39" name="图片 38"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="10315575"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>350917</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>341392</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="40" name="图片 39"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="161925" y="10106025"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2406,8 +2482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3063,6 +3139,9 @@
       </c>
       <c r="F34" s="2">
         <v>54</v>
+      </c>
+      <c r="G34" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="17.25" thickBot="1">

</xml_diff>

<commit_message>
add 1545 1496 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="162">
   <si>
     <t>ID</t>
   </si>
@@ -499,6 +499,14 @@
   </si>
   <si>
     <t>*</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -2295,6 +2303,196 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="209550" y="11153775"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>389017</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>198517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="图片 43"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="200025" y="12744450"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>408067</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>217567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="图片 44"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="219075" y="12544425"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>379492</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>360442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="图片 45"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="190500" y="11506200"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>417592</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>208042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="图片 46"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="12096750"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>417592</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>217567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="图片 47"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="228600" y="12325350"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2596,8 +2794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3371,6 +3569,9 @@
       <c r="F40" s="2">
         <v>56</v>
       </c>
+      <c r="G40" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="41" spans="1:7" ht="17.25" thickBot="1">
       <c r="A41" s="2"/>
@@ -3425,6 +3626,9 @@
       <c r="F43" s="2">
         <v>61</v>
       </c>
+      <c r="G43" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="44" spans="1:7" ht="17.25" thickBot="1">
       <c r="A44" s="2"/>
@@ -3460,6 +3664,9 @@
       </c>
       <c r="F45" s="2">
         <v>61</v>
+      </c>
+      <c r="G45" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="29.25" thickBot="1">
@@ -4582,8 +4789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D1"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D47" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
add 1224 1617 2056 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="166">
   <si>
     <t>ID</t>
   </si>
@@ -507,6 +507,18 @@
   </si>
   <si>
     <t>?</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>*</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>?</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>？</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
@@ -2589,6 +2601,120 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="219075" y="11849100"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>436642</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>188992</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="图片 50"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="14354175"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>436642</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>188992</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="图片 51"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="14944725"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>398542</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>322342</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="图片 52"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="209550" y="16478250"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2890,8 +3016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -3801,6 +3927,9 @@
       <c r="F47" s="2">
         <v>64</v>
       </c>
+      <c r="G47" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="48" spans="1:7" ht="17.25" thickBot="1">
       <c r="A48" s="2"/>
@@ -3820,7 +3949,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="29.25" thickBot="1">
+    <row r="49" spans="1:7" ht="29.25" thickBot="1">
       <c r="A49" s="2"/>
       <c r="B49" s="2">
         <v>1654</v>
@@ -3837,8 +3966,11 @@
       <c r="F49" s="2">
         <v>65</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="17.25" thickBot="1">
+      <c r="G49" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="17.25" thickBot="1">
       <c r="A50" s="2"/>
       <c r="B50" s="2">
         <v>1617</v>
@@ -3856,7 +3988,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="29.25" thickBot="1">
+    <row r="51" spans="1:7" ht="29.25" thickBot="1">
       <c r="A51" s="2"/>
       <c r="B51" s="2">
         <v>1723</v>
@@ -3874,7 +4006,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="17.25" thickBot="1">
+    <row r="52" spans="1:7" ht="17.25" thickBot="1">
       <c r="A52" s="2"/>
       <c r="B52" s="2">
         <v>2056</v>
@@ -3892,7 +4024,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="17.25" thickBot="1">
+    <row r="53" spans="1:7" ht="17.25" thickBot="1">
       <c r="A53" s="2"/>
       <c r="B53" s="2">
         <v>1131</v>
@@ -3909,8 +4041,11 @@
       <c r="F53" s="2">
         <v>69</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="29.25" thickBot="1">
+      <c r="G53" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="29.25" thickBot="1">
       <c r="A54" s="2"/>
       <c r="B54" s="2">
         <v>2002</v>
@@ -3928,7 +4063,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="1:6" ht="29.25" thickBot="1">
+    <row r="55" spans="1:7" ht="29.25" thickBot="1">
       <c r="A55" s="2"/>
       <c r="B55" s="2">
         <v>2035</v>
@@ -3946,7 +4081,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="17.25" thickBot="1">
+    <row r="56" spans="1:7" ht="17.25" thickBot="1">
       <c r="A56" s="2"/>
       <c r="B56" s="2">
         <v>1025</v>
@@ -3964,7 +4099,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="29.25" thickBot="1">
+    <row r="57" spans="1:7" ht="29.25" thickBot="1">
       <c r="A57" s="2"/>
       <c r="B57" s="2">
         <v>1224</v>
@@ -3981,8 +4116,11 @@
       <c r="F57" s="2">
         <v>70</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" ht="29.25" thickBot="1">
+      <c r="G57" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="29.25" thickBot="1">
       <c r="A58" s="2"/>
       <c r="B58" s="2">
         <v>1457</v>
@@ -4000,7 +4138,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:6" ht="17.25" thickBot="1">
+    <row r="59" spans="1:7" ht="17.25" thickBot="1">
       <c r="A59" s="2"/>
       <c r="B59" s="2">
         <v>1083</v>
@@ -4018,7 +4156,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="60" spans="1:6" ht="17.25" thickBot="1">
+    <row r="60" spans="1:7" ht="17.25" thickBot="1">
       <c r="A60" s="2"/>
       <c r="B60" s="2">
         <v>1935</v>
@@ -4036,7 +4174,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="29.25" thickBot="1">
+    <row r="61" spans="1:7" ht="29.25" thickBot="1">
       <c r="A61" s="2"/>
       <c r="B61" s="2">
         <v>1792</v>
@@ -4054,7 +4192,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="29.25" thickBot="1">
+    <row r="62" spans="1:7" ht="29.25" thickBot="1">
       <c r="A62" s="2"/>
       <c r="B62" s="2">
         <v>2005</v>
@@ -4072,7 +4210,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="29.25" thickBot="1">
+    <row r="63" spans="1:7" ht="29.25" thickBot="1">
       <c r="A63" s="2"/>
       <c r="B63" s="2">
         <v>2031</v>
@@ -4090,7 +4228,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="29.25" thickBot="1">
+    <row r="64" spans="1:7" ht="29.25" thickBot="1">
       <c r="A64" s="2"/>
       <c r="B64" s="2">
         <v>1502</v>

</xml_diff>

<commit_message>
add 1638 1404 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -2913,6 +2913,82 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="247650" y="13544550"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>408067</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>208042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="图片 58"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="219075" y="19030950"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>360442</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>198517</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="图片 59"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="21755100"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3214,8 +3290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
add 1118 2033 result
</commit_message>
<xml_diff>
--- a/ural 100.xlsx
+++ b/ural 100.xlsx
@@ -2989,6 +2989,82 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="171450" y="21755100"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>436642</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>322342</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="图片 60"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="27612975"/>
+          <a:ext cx="188992" cy="188992"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>436642</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>208042</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="图片 61"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="247650" y="27870150"/>
           <a:ext cx="188992" cy="188992"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3290,8 +3366,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>